<commit_message>
Aggiunti due file Uno per gli step fatti e da fare Uno per scrivere le soluzioni
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -95,7 +95,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -138,12 +138,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -323,7 +317,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -392,10 +386,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -420,7 +410,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -552,16 +542,16 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3:T3"/>
+      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="4.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="4.52"/>
@@ -624,305 +614,305 @@
       <c r="J3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="17" t="n">
+      <c r="M3" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N3" s="17" t="n">
+      <c r="N3" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="O3" s="17" t="n">
+      <c r="O3" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="P3" s="17" t="n">
+      <c r="P3" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="Q3" s="17" t="n">
+      <c r="Q3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="R3" s="17" t="n">
+      <c r="R3" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="S3" s="17" t="n">
+      <c r="S3" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="T3" s="17" t="n">
+      <c r="T3" s="0" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="19" t="n">
+      <c r="B4" s="18" t="n">
         <v>139</v>
       </c>
-      <c r="C4" s="20" t="n">
+      <c r="C4" s="19" t="n">
         <v>611</v>
       </c>
-      <c r="D4" s="20" t="n">
+      <c r="D4" s="19" t="n">
         <v>5751</v>
       </c>
-      <c r="E4" s="20" t="n">
+      <c r="E4" s="19" t="n">
         <v>13</v>
       </c>
-      <c r="F4" s="20" t="n">
+      <c r="F4" s="19" t="n">
         <v>0.14</v>
       </c>
-      <c r="G4" s="21" t="n">
+      <c r="G4" s="20" t="n">
         <v>157.032733</v>
       </c>
-      <c r="I4" s="22" t="n">
+      <c r="I4" s="21" t="n">
         <f aca="false">AVERAGE(M4:M2000)</f>
         <v>157.929623</v>
       </c>
-      <c r="J4" s="23" t="n">
+      <c r="J4" s="22" t="n">
         <f aca="false">100*(I4-G4)/G4</f>
         <v>0.571148436931289</v>
       </c>
-      <c r="M4" s="24" t="n">
+      <c r="M4" s="23" t="n">
         <v>157.929623</v>
       </c>
-      <c r="N4" s="24" t="n">
-        <v>42.7715196599</v>
-      </c>
-      <c r="O4" s="24" t="n">
+      <c r="N4" s="23" t="n">
+        <v>42.771519659</v>
+      </c>
+      <c r="O4" s="23" t="n">
         <v>47.53688888</v>
       </c>
-      <c r="P4" s="24" t="n">
+      <c r="P4" s="23" t="n">
         <v>10.156422</v>
       </c>
-      <c r="Q4" s="24" t="n">
+      <c r="Q4" s="23" t="n">
         <v>18.05870256</v>
       </c>
-      <c r="R4" s="24" t="n">
+      <c r="R4" s="23" t="n">
         <v>6.154801</v>
       </c>
-      <c r="S4" s="24" t="n">
+      <c r="S4" s="23" t="n">
         <v>12.54339552</v>
       </c>
-      <c r="T4" s="24" t="n">
+      <c r="T4" s="23" t="n">
         <v>26.312477</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="26" t="n">
+      <c r="B5" s="25" t="n">
         <v>181</v>
       </c>
-      <c r="C5" s="27" t="n">
+      <c r="C5" s="26" t="n">
         <v>941</v>
       </c>
-      <c r="D5" s="27" t="n">
+      <c r="D5" s="26" t="n">
         <v>6034</v>
       </c>
-      <c r="E5" s="27" t="n">
+      <c r="E5" s="26" t="n">
         <v>21</v>
       </c>
-      <c r="F5" s="27" t="n">
+      <c r="F5" s="26" t="n">
         <v>0.29</v>
       </c>
-      <c r="G5" s="28" t="n">
+      <c r="G5" s="27" t="n">
         <v>34.70882</v>
       </c>
-      <c r="I5" s="29" t="n">
+      <c r="I5" s="28" t="n">
         <f aca="false">AVERAGE(N4:N2000)</f>
-        <v>42.7715196599</v>
-      </c>
-      <c r="J5" s="30" t="n">
+        <v>42.771519659</v>
+      </c>
+      <c r="J5" s="29" t="n">
         <f aca="false">100*(I5-G5)/G5</f>
-        <v>23.2295412517625</v>
+        <v>23.2295412491695</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="26" t="n">
+      <c r="B6" s="25" t="n">
         <v>190</v>
       </c>
-      <c r="C6" s="27" t="n">
+      <c r="C6" s="26" t="n">
         <v>1125</v>
       </c>
-      <c r="D6" s="27" t="n">
+      <c r="D6" s="26" t="n">
         <v>8109</v>
       </c>
-      <c r="E6" s="27" t="n">
+      <c r="E6" s="26" t="n">
         <v>24</v>
       </c>
-      <c r="F6" s="27" t="n">
+      <c r="F6" s="26" t="n">
         <v>0.27</v>
       </c>
-      <c r="G6" s="28" t="n">
+      <c r="G6" s="27" t="n">
         <v>32.626667</v>
       </c>
-      <c r="I6" s="29" t="n">
+      <c r="I6" s="28" t="n">
         <f aca="false">AVERAGE(O4:O2000)</f>
         <v>47.53688888</v>
       </c>
-      <c r="J6" s="30" t="n">
+      <c r="J6" s="29" t="n">
         <f aca="false">100*(I6-G6)/G6</f>
         <v>45.6994944656774</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="26" t="n">
+      <c r="B7" s="25" t="n">
         <v>261</v>
       </c>
-      <c r="C7" s="27" t="n">
+      <c r="C7" s="26" t="n">
         <v>4360</v>
       </c>
-      <c r="D7" s="27" t="n">
+      <c r="D7" s="26" t="n">
         <v>14901</v>
       </c>
-      <c r="E7" s="27" t="n">
+      <c r="E7" s="26" t="n">
         <v>23</v>
       </c>
-      <c r="F7" s="27" t="n">
+      <c r="F7" s="26" t="n">
         <v>0.18</v>
       </c>
-      <c r="G7" s="28" t="n">
+      <c r="G7" s="27" t="n">
         <v>7.717202</v>
       </c>
-      <c r="I7" s="29" t="n">
+      <c r="I7" s="28" t="n">
         <f aca="false">AVERAGE(P4:P2000)</f>
         <v>10.156422</v>
       </c>
-      <c r="J7" s="30" t="n">
+      <c r="J7" s="29" t="n">
         <f aca="false">100*(I7-G7)/G7</f>
         <v>31.6075696865263</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="26" t="n">
+      <c r="B8" s="25" t="n">
         <v>461</v>
       </c>
-      <c r="C8" s="27" t="n">
+      <c r="C8" s="26" t="n">
         <v>5349</v>
       </c>
-      <c r="D8" s="27" t="n">
+      <c r="D8" s="26" t="n">
         <v>25113</v>
       </c>
-      <c r="E8" s="27" t="n">
+      <c r="E8" s="26" t="n">
         <v>20</v>
       </c>
-      <c r="F8" s="27" t="n">
+      <c r="F8" s="26" t="n">
         <v>0.06</v>
       </c>
-      <c r="G8" s="28" t="n">
+      <c r="G8" s="27" t="n">
         <v>12.901103</v>
       </c>
-      <c r="I8" s="29" t="n">
+      <c r="I8" s="28" t="n">
         <f aca="false">AVERAGE(Q4:Q2000)</f>
         <v>18.05870256</v>
       </c>
-      <c r="J8" s="30" t="n">
+      <c r="J8" s="29" t="n">
         <f aca="false">100*(I8-G8)/G8</f>
         <v>39.9779736662826</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="26" t="n">
+      <c r="B9" s="25" t="n">
         <v>622</v>
       </c>
-      <c r="C9" s="27" t="n">
+      <c r="C9" s="26" t="n">
         <v>21266</v>
       </c>
-      <c r="D9" s="27" t="n">
+      <c r="D9" s="26" t="n">
         <v>58979</v>
       </c>
-      <c r="E9" s="27" t="n">
+      <c r="E9" s="26" t="n">
         <v>35</v>
       </c>
-      <c r="F9" s="27" t="n">
+      <c r="F9" s="26" t="n">
         <v>0.13</v>
       </c>
-      <c r="G9" s="28" t="n">
+      <c r="G9" s="27" t="n">
         <v>3.044578</v>
       </c>
-      <c r="I9" s="29" t="n">
+      <c r="I9" s="28" t="n">
         <f aca="false">AVERAGE(R4:R2000)</f>
         <v>6.154801</v>
       </c>
-      <c r="J9" s="30" t="n">
+      <c r="J9" s="29" t="n">
         <f aca="false">100*(I9-G9)/G9</f>
         <v>102.15612804139</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="26" t="n">
+      <c r="B10" s="25" t="n">
         <v>81</v>
       </c>
-      <c r="C10" s="27" t="n">
+      <c r="C10" s="26" t="n">
         <v>2823</v>
       </c>
-      <c r="D10" s="27" t="n">
+      <c r="D10" s="26" t="n">
         <v>10632</v>
       </c>
-      <c r="E10" s="27" t="n">
+      <c r="E10" s="26" t="n">
         <v>18</v>
       </c>
-      <c r="F10" s="27" t="n">
+      <c r="F10" s="26" t="n">
         <v>0.42</v>
       </c>
-      <c r="G10" s="28" t="n">
+      <c r="G10" s="27" t="n">
         <v>10.050301</v>
       </c>
-      <c r="I10" s="29" t="n">
+      <c r="I10" s="28" t="n">
         <f aca="false">AVERAGE(S4:S2000)</f>
         <v>12.54339552</v>
       </c>
-      <c r="J10" s="30" t="n">
+      <c r="J10" s="29" t="n">
         <f aca="false">100*(I10-G10)/G10</f>
         <v>24.806167695873</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="32" t="n">
+      <c r="B11" s="31" t="n">
         <v>184</v>
       </c>
-      <c r="C11" s="33" t="n">
+      <c r="C11" s="32" t="n">
         <v>2750</v>
       </c>
-      <c r="D11" s="33" t="n">
+      <c r="D11" s="32" t="n">
         <v>11793</v>
       </c>
-      <c r="E11" s="33" t="n">
+      <c r="E11" s="32" t="n">
         <v>10</v>
       </c>
-      <c r="F11" s="33" t="n">
+      <c r="F11" s="32" t="n">
         <v>0.08</v>
       </c>
-      <c r="G11" s="34" t="n">
+      <c r="G11" s="33" t="n">
         <v>24.769</v>
       </c>
-      <c r="I11" s="29" t="n">
+      <c r="I11" s="28" t="n">
         <f aca="false">AVERAGE(T4:T2000)</f>
         <v>26.312477</v>
       </c>
-      <c r="J11" s="35" t="n">
+      <c r="J11" s="34" t="n">
         <f aca="false">100*(I11-G11)/G11</f>
         <v>6.23148693931932</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="36" t="s">
+      <c r="I13" s="35" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="2" t="n">
@@ -931,16 +921,16 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I14" s="36" t="s">
+      <c r="I14" s="35" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="2" t="n">
         <f aca="false">AVERAGE(J4:J11)</f>
-        <v>34.2849387729703</v>
+        <v>34.2849387726462</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I15" s="36" t="s">
+      <c r="I15" s="35" t="s">
         <v>20</v>
       </c>
       <c r="J15" s="2" t="n">

</xml_diff>

<commit_message>
Ho inserito una tabulist sulla sezione di taglio e sul rinnovo popolazione considero anche il tempo trascorso dall'ultimo miglioramento. Pare migliorare ma non ne sono sicuro
</commit_message>
<xml_diff>
--- a/benchmarks.xlsx
+++ b/benchmarks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simone/git/DMO_proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B4B8ED-1C8C-804A-BA13-E4631CE6E0E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA62C5BD-8DA3-1E41-AE45-06DD8F4B9E0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -839,12 +839,12 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5:U5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.5" customWidth="1"/>
     <col min="2" max="2" width="5.5" customWidth="1"/>
     <col min="3" max="3" width="6.5" customWidth="1"/>
     <col min="4" max="4" width="6.6640625" customWidth="1"/>
@@ -1015,20 +1015,20 @@
       </c>
       <c r="I5" s="28">
         <f>AVERAGE(N4:N2000)</f>
-        <v>43.235759829499997</v>
+        <v>42.830759829499996</v>
       </c>
       <c r="J5" s="29">
         <f t="shared" si="0"/>
-        <v>24.567069204599854</v>
+        <v>23.400218819020619</v>
       </c>
       <c r="M5" s="36">
         <v>157.4</v>
       </c>
       <c r="N5" s="36">
-        <v>43.7</v>
+        <v>42.89</v>
       </c>
       <c r="O5" s="36">
-        <v>42.3</v>
+        <v>40.79</v>
       </c>
       <c r="P5" s="36">
         <v>9.6999999999999993</v>
@@ -1040,7 +1040,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="S5" s="36">
-        <v>11.5</v>
+        <v>11.32</v>
       </c>
       <c r="T5" s="36">
         <v>26.9</v>
@@ -1073,11 +1073,11 @@
       </c>
       <c r="I6" s="28">
         <f>AVERAGE(O4:O2000)</f>
-        <v>44.918444440000002</v>
+        <v>44.163444439999999</v>
       </c>
       <c r="J6" s="29">
         <f t="shared" si="0"/>
-        <v>37.674021192541687</v>
+        <v>35.359963185942348</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -1197,11 +1197,11 @@
       </c>
       <c r="I10" s="28">
         <f>AVERAGE(S4:S2000)</f>
-        <v>12.02169776</v>
+        <v>11.93169776</v>
       </c>
       <c r="J10" s="29">
         <f t="shared" si="0"/>
-        <v>19.615300676069317</v>
+        <v>18.719805108324628</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -1250,7 +1250,7 @@
       </c>
       <c r="J14" s="2">
         <f>AVERAGE(J4:J11)</f>
-        <v>28.345519989030667</v>
+        <v>27.798469494040258</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">

</xml_diff>